<commit_message>
updated cotton observed files
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/Emerald2015Observed.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/Emerald2015Observed.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F0191E-F88C-4830-A490-0A39391A27CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9D63FC-8804-4E6C-81B2-11FE3328729D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{3150B938-1320-42B8-B855-5DFCB1CA6EF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3150B938-1320-42B8-B855-5DFCB1CA6EF9}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
     <sheet name="PhenologyObserved" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$Y$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$Z$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="46">
   <si>
     <t>SimulationName</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Cotton.Phenology.EmergenceDAS</t>
+  </si>
+  <si>
+    <t>Cotton.SeedCotton.Wt</t>
   </si>
 </sst>
 </file>
@@ -554,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7F552A-40E4-417F-B0AA-493C63AE000C}">
-  <dimension ref="A1:Y51"/>
+  <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -575,25 +578,26 @@
     <col min="8" max="8" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="5"/>
+    <col min="11" max="11" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -624,53 +628,56 @@
       <c r="J1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -697,14 +704,12 @@
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="K2" s="5"/>
       <c r="Q2" s="4"/>
-      <c r="Y2" s="8"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R2" s="4"/>
+      <c r="Z2" s="8"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -728,44 +733,35 @@
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="O3" s="6">
+      <c r="K3" s="5"/>
+      <c r="P3" s="6">
         <v>6.0500000000000007</v>
       </c>
-      <c r="P3" s="5">
+      <c r="Q3" s="5">
         <v>6.0256249999999997E-2</v>
       </c>
-      <c r="Q3" s="7">
-        <f>P3/O3</f>
+      <c r="R3" s="7">
+        <f>Q3/P3</f>
         <v>9.9597107438016506E-3</v>
       </c>
-      <c r="R3" s="6">
+      <c r="S3" s="6">
         <v>2.8187499999999996</v>
       </c>
-      <c r="S3" s="6">
-        <v>0</v>
-      </c>
-      <c r="T3" s="6">
-        <f>SUM(O3:S3)</f>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6">
+        <f>SUM(P3:T3)</f>
         <v>8.9389659607438023</v>
       </c>
-      <c r="U3" s="5">
-        <f>R3/T3</f>
+      <c r="V3" s="5">
+        <f>S3/U3</f>
         <v>0.31533289335464193</v>
       </c>
-      <c r="V3" s="5">
-        <f>O3/T3</f>
+      <c r="W3" s="5">
+        <f>P3/U3</f>
         <v>0.67681206378557301</v>
       </c>
-      <c r="W3" s="5">
-        <f>S3/T3</f>
-        <v>0</v>
-      </c>
-      <c r="X3" s="5">
-        <f>S3/T3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -782,12 +778,13 @@
       <c r="J4" s="2">
         <v>4.8499999999999996</v>
       </c>
-      <c r="K4"/>
-      <c r="O4"/>
-      <c r="Q4"/>
-      <c r="U4"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="P4"/>
+      <c r="R4"/>
+      <c r="V4"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -804,12 +801,13 @@
       <c r="J5" s="2">
         <v>8.8000000000000007</v>
       </c>
-      <c r="K5"/>
-      <c r="O5"/>
-      <c r="Q5"/>
-      <c r="U5"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="P5"/>
+      <c r="R5"/>
+      <c r="V5"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -836,44 +834,45 @@
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="O6" s="6">
+      <c r="K6" s="5"/>
+      <c r="P6" s="6">
         <v>24.15</v>
       </c>
-      <c r="P6" s="5">
+      <c r="Q6" s="5">
         <v>0.23917499999999994</v>
       </c>
-      <c r="Q6" s="7">
-        <f>P6/O6</f>
+      <c r="R6" s="7">
+        <f>Q6/P6</f>
         <v>9.9037267080745329E-3</v>
       </c>
-      <c r="R6" s="6">
+      <c r="S6" s="6">
         <v>18.462499999999999</v>
       </c>
-      <c r="S6" s="6">
+      <c r="T6" s="6">
         <v>2.4736039515622594</v>
       </c>
-      <c r="T6" s="6">
-        <f>SUM(O6:S6)</f>
+      <c r="U6" s="6">
+        <f>SUM(P6:T6)</f>
         <v>45.335182678270336</v>
       </c>
-      <c r="U6" s="5">
-        <f>R6/T6</f>
+      <c r="V6" s="5">
+        <f>S6/U6</f>
         <v>0.40724441613090229</v>
       </c>
-      <c r="V6" s="5">
-        <f>O6/T6</f>
+      <c r="W6" s="5">
+        <f>P6/U6</f>
         <v>0.53269885711909493</v>
       </c>
-      <c r="W6" s="5">
-        <f>S6/T6</f>
+      <c r="X6" s="5">
+        <f>T6/U6</f>
         <v>5.4562567203415853E-2</v>
       </c>
-      <c r="X6" s="5">
-        <f>S6/T6</f>
+      <c r="Y6" s="5">
+        <f>T6/U6</f>
         <v>5.4562567203415853E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -890,12 +889,13 @@
       <c r="J7" s="2">
         <v>10.775</v>
       </c>
-      <c r="K7"/>
-      <c r="O7"/>
-      <c r="Q7"/>
-      <c r="U7"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="P7"/>
+      <c r="R7"/>
+      <c r="V7"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -914,12 +914,13 @@
       <c r="J8" s="2">
         <v>14.475</v>
       </c>
-      <c r="K8"/>
-      <c r="O8"/>
-      <c r="Q8"/>
-      <c r="U8"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="P8"/>
+      <c r="R8"/>
+      <c r="V8"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -946,44 +947,45 @@
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="O9" s="6">
+      <c r="K9" s="5"/>
+      <c r="P9" s="6">
         <v>85.802005610261531</v>
       </c>
-      <c r="P9" s="5">
+      <c r="Q9" s="5">
         <v>1.2492019355377233</v>
       </c>
-      <c r="Q9" s="7">
-        <f>P9/O9</f>
+      <c r="R9" s="7">
+        <f>Q9/P9</f>
         <v>1.455912279267659E-2</v>
       </c>
-      <c r="R9" s="6">
+      <c r="S9" s="6">
         <v>83.77238281861348</v>
       </c>
-      <c r="S9" s="6">
+      <c r="T9" s="6">
         <v>14.841623709373557</v>
       </c>
-      <c r="T9" s="6">
-        <f>SUM(O9:S9)</f>
+      <c r="U9" s="6">
+        <f>SUM(P9:T9)</f>
         <v>185.67977319657896</v>
       </c>
-      <c r="U9" s="5">
-        <f>R9/T9</f>
+      <c r="V9" s="5">
+        <f>S9/U9</f>
         <v>0.45116590448397281</v>
       </c>
-      <c r="V9" s="5">
-        <f>O9/T9</f>
+      <c r="W9" s="5">
+        <f>P9/U9</f>
         <v>0.46209667393024573</v>
       </c>
-      <c r="W9" s="5">
-        <f>S9/T9</f>
+      <c r="X9" s="5">
+        <f>T9/U9</f>
         <v>7.9931289519945437E-2</v>
       </c>
-      <c r="X9" s="5">
-        <f>S9/T9</f>
+      <c r="Y9" s="5">
+        <f>T9/U9</f>
         <v>7.9931289519945437E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1002,12 +1004,13 @@
       <c r="J10" s="2">
         <v>16.95</v>
       </c>
-      <c r="K10"/>
-      <c r="O10"/>
-      <c r="Q10"/>
-      <c r="U10"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="P10"/>
+      <c r="R10"/>
+      <c r="V10"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -1026,12 +1029,13 @@
       <c r="J11" s="2">
         <v>20.05</v>
       </c>
-      <c r="K11"/>
-      <c r="O11"/>
-      <c r="Q11"/>
-      <c r="U11"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="P11"/>
+      <c r="R11"/>
+      <c r="V11"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
@@ -1059,44 +1063,45 @@
       <c r="J12" s="2">
         <v>21.524999999999999</v>
       </c>
-      <c r="O12" s="6">
+      <c r="K12" s="1"/>
+      <c r="P12" s="6">
         <v>226.26821947863289</v>
       </c>
-      <c r="P12" s="5">
+      <c r="Q12" s="5">
         <v>2.7797532561653497</v>
       </c>
-      <c r="Q12" s="7">
-        <f>P12/O12</f>
+      <c r="R12" s="7">
+        <f>Q12/P12</f>
         <v>1.2285212932556131E-2</v>
       </c>
-      <c r="R12" s="6">
+      <c r="S12" s="6">
         <v>285.33279165649009</v>
       </c>
-      <c r="S12" s="6">
+      <c r="T12" s="6">
         <v>114.02173814823612</v>
       </c>
-      <c r="T12" s="6">
-        <f>SUM(O12:S12)</f>
+      <c r="U12" s="6">
+        <f>SUM(P12:T12)</f>
         <v>628.41478775245696</v>
       </c>
-      <c r="U12" s="5">
-        <f>R12/T12</f>
+      <c r="V12" s="5">
+        <f>S12/U12</f>
         <v>0.45405168245163485</v>
       </c>
-      <c r="V12" s="5">
-        <f>O12/T12</f>
+      <c r="W12" s="5">
+        <f>P12/U12</f>
         <v>0.36006189524579379</v>
       </c>
-      <c r="W12" s="5">
-        <f>S12/T12</f>
+      <c r="X12" s="5">
+        <f>T12/U12</f>
         <v>0.18144343572187099</v>
       </c>
-      <c r="X12" s="5">
-        <f>S12/T12</f>
+      <c r="Y12" s="5">
+        <f>T12/U12</f>
         <v>0.18144343572187099</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1115,12 +1120,13 @@
       <c r="J13" s="2">
         <v>21.6</v>
       </c>
-      <c r="K13"/>
-      <c r="O13"/>
-      <c r="Q13"/>
-      <c r="U13"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="P13"/>
+      <c r="R13"/>
+      <c r="V13"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -1151,44 +1157,45 @@
       <c r="J14" s="2">
         <v>22.524999999999999</v>
       </c>
-      <c r="O14" s="6">
+      <c r="K14" s="1"/>
+      <c r="P14" s="6">
         <v>188.90327142068634</v>
       </c>
-      <c r="P14" s="5">
+      <c r="Q14" s="5">
         <v>3.1133432138518815</v>
       </c>
-      <c r="Q14" s="7">
-        <f>P14/O14</f>
+      <c r="R14" s="7">
+        <f>Q14/P14</f>
         <v>1.6481150328617057E-2</v>
       </c>
-      <c r="R14" s="6">
+      <c r="S14" s="6">
         <v>261.39276028775987</v>
       </c>
-      <c r="S14" s="6">
+      <c r="T14" s="6">
         <v>399.91574599674937</v>
       </c>
-      <c r="T14" s="6">
-        <f>SUM(O14:S14)</f>
+      <c r="U14" s="6">
+        <f>SUM(P14:T14)</f>
         <v>853.34160206937611</v>
       </c>
-      <c r="U14" s="5">
-        <f>R14/T14</f>
+      <c r="V14" s="5">
+        <f>S14/U14</f>
         <v>0.30631667277661778</v>
       </c>
-      <c r="V14" s="5">
-        <f>O14/T14</f>
+      <c r="W14" s="5">
+        <f>P14/U14</f>
         <v>0.2213688761482985</v>
       </c>
-      <c r="W14" s="5">
-        <f>S14/T14</f>
+      <c r="X14" s="5">
+        <f>T14/U14</f>
         <v>0.46864672368831312</v>
       </c>
-      <c r="X14" s="5">
-        <f>S14/T14</f>
+      <c r="Y14" s="5">
+        <f>T14/U14</f>
         <v>0.46864672368831312</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
@@ -1215,44 +1222,45 @@
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-      <c r="O15" s="6">
+      <c r="K15" s="5"/>
+      <c r="P15" s="6">
         <v>196.30959768735224</v>
       </c>
-      <c r="P15" s="5">
+      <c r="Q15" s="5">
         <v>3.121836139804687</v>
       </c>
-      <c r="Q15" s="7">
-        <f>P15/O15</f>
+      <c r="R15" s="7">
+        <f>Q15/P15</f>
         <v>1.5902615952464047E-2</v>
       </c>
-      <c r="R15" s="6">
+      <c r="S15" s="6">
         <v>280.3496253427212</v>
       </c>
-      <c r="S15" s="6">
+      <c r="T15" s="6">
         <v>629.08253602487207</v>
       </c>
-      <c r="T15" s="6">
-        <f>SUM(O15:S15)</f>
+      <c r="U15" s="6">
+        <f>SUM(P15:T15)</f>
         <v>1108.8794978107026</v>
       </c>
-      <c r="U15" s="5">
-        <f>R15/T15</f>
+      <c r="V15" s="5">
+        <f>S15/U15</f>
         <v>0.25282244454534936</v>
       </c>
-      <c r="V15" s="5">
-        <f>O15/T15</f>
+      <c r="W15" s="5">
+        <f>P15/U15</f>
         <v>0.17703420261167491</v>
       </c>
-      <c r="W15" s="5">
-        <f>S15/T15</f>
+      <c r="X15" s="5">
+        <f>T15/U15</f>
         <v>0.56731370475050757</v>
       </c>
-      <c r="X15" s="5">
-        <f>S15/T15</f>
+      <c r="Y15" s="5">
+        <f>T15/U15</f>
         <v>0.56731370475050757</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1279,44 +1287,45 @@
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="O16" s="6">
+      <c r="K16" s="5"/>
+      <c r="P16" s="6">
         <v>226.84774664880791</v>
       </c>
-      <c r="P16" s="5">
+      <c r="Q16" s="5">
         <v>2.6258533911366184</v>
       </c>
-      <c r="Q16" s="7">
-        <f>P16/O16</f>
+      <c r="R16" s="7">
+        <f>Q16/P16</f>
         <v>1.1575399932016108E-2</v>
       </c>
-      <c r="R16" s="6">
+      <c r="S16" s="6">
         <v>346.94008009677322</v>
       </c>
-      <c r="S16" s="6">
+      <c r="T16" s="6">
         <v>803.9944254839686</v>
       </c>
-      <c r="T16" s="6">
-        <f>SUM(O16:S16)</f>
+      <c r="U16" s="6">
+        <f>SUM(P16:T16)</f>
         <v>1380.4196810206183</v>
       </c>
-      <c r="U16" s="5">
-        <f>R16/T16</f>
+      <c r="V16" s="5">
+        <f>S16/U16</f>
         <v>0.2513294216728798</v>
       </c>
-      <c r="V16" s="5">
-        <f>O16/T16</f>
+      <c r="W16" s="5">
+        <f>P16/U16</f>
         <v>0.16433244886880141</v>
       </c>
-      <c r="W16" s="5">
-        <f>S16/T16</f>
+      <c r="X16" s="5">
+        <f>T16/U16</f>
         <v>0.58242753022003602</v>
       </c>
-      <c r="X16" s="5">
-        <f>S16/T16</f>
+      <c r="Y16" s="5">
+        <f>T16/U16</f>
         <v>0.58242753022003602</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -1343,23 +1352,28 @@
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="4">
+      <c r="K17" s="5">
+        <v>722.44939607169499</v>
+      </c>
+      <c r="L17" s="5">
         <v>44.449999999999989</v>
       </c>
-      <c r="L17" s="5">
+      <c r="M17" s="5">
         <v>321.12875655386836</v>
       </c>
-      <c r="M17" s="4"/>
-      <c r="N17" s="8">
+      <c r="N17" s="5">
+        <v>401.32063951782663</v>
+      </c>
+      <c r="O17" s="5">
         <v>14.146641257879665</v>
       </c>
-      <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
-      <c r="Y17" s="8">
+      <c r="R17" s="8"/>
+      <c r="Z17" s="8">
         <v>129.19999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -1386,10 +1400,10 @@
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-      <c r="M18" s="4"/>
-      <c r="Y18" s="8"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K18" s="5"/>
+      <c r="Z18" s="8"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -1415,44 +1429,35 @@
       <c r="J19" s="2">
         <v>5.75</v>
       </c>
-      <c r="O19" s="10">
+      <c r="K19" s="1"/>
+      <c r="P19" s="10">
         <v>10.056249999999999</v>
       </c>
-      <c r="P19" s="11">
+      <c r="Q19" s="11">
         <v>0.10627500000000001</v>
       </c>
-      <c r="Q19" s="7">
-        <f>P19/O19</f>
+      <c r="R19" s="7">
+        <f>Q19/P19</f>
         <v>1.0568054692355503E-2</v>
       </c>
-      <c r="R19" s="10">
+      <c r="S19" s="10">
         <v>4.6375000000000002</v>
       </c>
-      <c r="S19" s="10">
-        <v>0</v>
-      </c>
-      <c r="T19" s="6">
-        <f>SUM(O19:S19)</f>
+      <c r="T19" s="10"/>
+      <c r="U19" s="6">
+        <f>SUM(P19:T19)</f>
         <v>14.810593054692355</v>
       </c>
-      <c r="U19" s="5">
-        <f>R19/T19</f>
+      <c r="V19" s="5">
+        <f>S19/U19</f>
         <v>0.31312047956990674</v>
       </c>
-      <c r="V19" s="5">
-        <f>O19/T19</f>
+      <c r="W19" s="5">
+        <f>P19/U19</f>
         <v>0.67899036607544461</v>
       </c>
-      <c r="W19" s="5">
-        <f>S19/T19</f>
-        <v>0</v>
-      </c>
-      <c r="X19" s="5">
-        <f>S19/T19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -1472,9 +1477,9 @@
       <c r="J20" s="2">
         <v>7.85</v>
       </c>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
@@ -1501,44 +1506,45 @@
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="O21" s="10">
+      <c r="K21" s="5"/>
+      <c r="P21" s="10">
         <v>21.65625</v>
       </c>
-      <c r="P21" s="11">
+      <c r="Q21" s="11">
         <v>0.27433750000000001</v>
       </c>
-      <c r="Q21" s="7">
-        <f>P21/O21</f>
+      <c r="R21" s="7">
+        <f>Q21/P21</f>
         <v>1.2667821067821069E-2</v>
       </c>
-      <c r="R21" s="10">
+      <c r="S21" s="10">
         <v>13.981250000000001</v>
       </c>
-      <c r="S21" s="10">
+      <c r="T21" s="10">
         <v>2.3421094856658908</v>
       </c>
-      <c r="T21" s="6">
-        <f>SUM(O21:S21)</f>
+      <c r="U21" s="6">
+        <f>SUM(P21:T21)</f>
         <v>38.26661480673372</v>
       </c>
-      <c r="U21" s="5">
-        <f>R21/T21</f>
+      <c r="V21" s="5">
+        <f>S21/U21</f>
         <v>0.3653641711087478</v>
       </c>
-      <c r="V21" s="5">
-        <f>O21/T21</f>
+      <c r="W21" s="5">
+        <f>P21/U21</f>
         <v>0.56593064501198531</v>
       </c>
-      <c r="W21" s="5">
-        <f>S21/T21</f>
+      <c r="X21" s="5">
+        <f>T21/U21</f>
         <v>6.120503466258409E-2</v>
       </c>
-      <c r="X21" s="5">
-        <f>S21/T21</f>
+      <c r="Y21" s="5">
+        <f>T21/U21</f>
         <v>6.120503466258409E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -1560,9 +1566,9 @@
       <c r="J22" s="2">
         <v>11.15</v>
       </c>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1584,8 +1590,9 @@
       <c r="J23" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1612,44 +1619,45 @@
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="O24" s="10">
+      <c r="K24" s="5"/>
+      <c r="P24" s="10">
         <v>94.668197908402803</v>
       </c>
-      <c r="P24" s="11">
+      <c r="Q24" s="11">
         <v>1.3627774023997914</v>
       </c>
-      <c r="Q24" s="7">
-        <f>P24/O24</f>
+      <c r="R24" s="7">
+        <f>Q24/P24</f>
         <v>1.4395303095537541E-2</v>
       </c>
-      <c r="R24" s="10">
+      <c r="S24" s="10">
         <v>87.153634995622809</v>
       </c>
-      <c r="S24" s="10">
+      <c r="T24" s="10">
         <v>14.052656913995346</v>
       </c>
-      <c r="T24" s="6">
-        <f>SUM(O24:S24)</f>
+      <c r="U24" s="6">
+        <f>SUM(P24:T24)</f>
         <v>197.2516625235163</v>
       </c>
-      <c r="U24" s="5">
-        <f>R24/T24</f>
+      <c r="V24" s="5">
+        <f>S24/U24</f>
         <v>0.44183979937422513</v>
       </c>
-      <c r="V24" s="5">
-        <f>O24/T24</f>
+      <c r="W24" s="5">
+        <f>P24/U24</f>
         <v>0.47993612168980571</v>
       </c>
-      <c r="W24" s="5">
-        <f>S24/T24</f>
+      <c r="X24" s="5">
+        <f>T24/U24</f>
         <v>7.1242273622509983E-2</v>
       </c>
-      <c r="X24" s="5">
-        <f>S24/T24</f>
+      <c r="Y24" s="5">
+        <f>T24/U24</f>
         <v>7.1242273622509983E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1671,8 +1679,9 @@
       <c r="J25" s="2">
         <v>18.149999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
@@ -1694,8 +1703,9 @@
       <c r="J26" s="2">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>18</v>
       </c>
@@ -1719,44 +1729,45 @@
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-      <c r="O27" s="10">
+      <c r="K27" s="5"/>
+      <c r="P27" s="10">
         <v>272.66068476775905</v>
       </c>
-      <c r="P27" s="11">
+      <c r="Q27" s="11">
         <v>3.0062498900225729</v>
       </c>
-      <c r="Q27" s="7">
-        <f>P27/O27</f>
+      <c r="R27" s="7">
+        <f>Q27/P27</f>
         <v>1.1025608230182398E-2</v>
       </c>
-      <c r="R27" s="10">
+      <c r="S27" s="10">
         <v>296.91054862314928</v>
       </c>
-      <c r="S27" s="10">
+      <c r="T27" s="10">
         <v>82.117764757664503</v>
       </c>
-      <c r="T27" s="6">
-        <f>SUM(O27:S27)</f>
+      <c r="U27" s="6">
+        <f>SUM(P27:T27)</f>
         <v>654.70627364682559</v>
       </c>
-      <c r="U27" s="5">
-        <f>R27/T27</f>
+      <c r="V27" s="5">
+        <f>S27/U27</f>
         <v>0.45350191463617251</v>
       </c>
-      <c r="V27" s="5">
-        <f>O27/T27</f>
+      <c r="W27" s="5">
+        <f>P27/U27</f>
         <v>0.41646261192670803</v>
       </c>
-      <c r="W27" s="5">
-        <f>S27/T27</f>
+      <c r="X27" s="5">
+        <f>T27/U27</f>
         <v>0.12542687929390769</v>
       </c>
-      <c r="X27" s="5">
-        <f>S27/T27</f>
+      <c r="Y27" s="5">
+        <f>T27/U27</f>
         <v>0.12542687929390769</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>18</v>
       </c>
@@ -1778,8 +1789,9 @@
       <c r="J28" s="2">
         <v>19.95</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>18</v>
       </c>
@@ -1801,8 +1813,9 @@
       <c r="J29" s="2">
         <v>22.1</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>18</v>
       </c>
@@ -1829,44 +1842,45 @@
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="O30" s="10">
+      <c r="K30" s="5"/>
+      <c r="P30" s="10">
         <v>199.00476263182486</v>
       </c>
-      <c r="P30" s="11">
+      <c r="Q30" s="11">
         <v>3.3243281303513257</v>
       </c>
-      <c r="Q30" s="7">
-        <f>P30/O30</f>
+      <c r="R30" s="7">
+        <f>Q30/P30</f>
         <v>1.6704766691949004E-2</v>
       </c>
-      <c r="R30" s="10">
+      <c r="S30" s="10">
         <v>256.44410342521178</v>
       </c>
-      <c r="S30" s="10">
+      <c r="T30" s="10">
         <v>337.14738531424558</v>
       </c>
-      <c r="T30" s="6">
-        <f>SUM(O30:S30)</f>
+      <c r="U30" s="6">
+        <f>SUM(P30:T30)</f>
         <v>795.93728426832558</v>
       </c>
-      <c r="U30" s="5">
-        <f>R30/T30</f>
+      <c r="V30" s="5">
+        <f>S30/U30</f>
         <v>0.32219134408429045</v>
       </c>
-      <c r="V30" s="5">
-        <f>O30/T30</f>
+      <c r="W30" s="5">
+        <f>P30/U30</f>
         <v>0.25002568238119699</v>
       </c>
-      <c r="W30" s="5">
-        <f>S30/T30</f>
+      <c r="X30" s="5">
+        <f>T30/U30</f>
         <v>0.42358536530195612</v>
       </c>
-      <c r="X30" s="5">
-        <f>S30/T30</f>
+      <c r="Y30" s="5">
+        <f>T30/U30</f>
         <v>0.42358536530195612</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>18</v>
       </c>
@@ -1888,8 +1902,9 @@
       <c r="J31" s="2">
         <v>23.9</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>18</v>
       </c>
@@ -1916,44 +1931,45 @@
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
-      <c r="O32" s="10">
+      <c r="K32" s="5"/>
+      <c r="P32" s="10">
         <v>219.92409364768787</v>
       </c>
-      <c r="P32" s="11">
+      <c r="Q32" s="11">
         <v>2.9603444754703503</v>
       </c>
-      <c r="Q32" s="7">
-        <f>P32/O32</f>
+      <c r="R32" s="7">
+        <f>Q32/P32</f>
         <v>1.3460755601488293E-2</v>
       </c>
-      <c r="R32" s="10">
+      <c r="S32" s="10">
         <v>248.95162430275457</v>
       </c>
-      <c r="S32" s="10">
+      <c r="T32" s="10">
         <v>607.699289545743</v>
       </c>
-      <c r="T32" s="6">
-        <f>SUM(O32:S32)</f>
+      <c r="U32" s="6">
+        <f>SUM(P32:T32)</f>
         <v>1079.5488127272574</v>
       </c>
-      <c r="U32" s="5">
-        <f>R32/T32</f>
+      <c r="V32" s="5">
+        <f>S32/U32</f>
         <v>0.2306071030487539</v>
       </c>
-      <c r="V32" s="5">
-        <f>O32/T32</f>
+      <c r="W32" s="5">
+        <f>P32/U32</f>
         <v>0.20371852671681887</v>
       </c>
-      <c r="W32" s="5">
-        <f>S32/T32</f>
+      <c r="X32" s="5">
+        <f>T32/U32</f>
         <v>0.56291969606313219</v>
       </c>
-      <c r="X32" s="5">
-        <f>S32/T32</f>
+      <c r="Y32" s="5">
+        <f>T32/U32</f>
         <v>0.56291969606313219</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>18</v>
       </c>
@@ -1980,44 +1996,45 @@
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
-      <c r="O33" s="10">
+      <c r="K33" s="5"/>
+      <c r="P33" s="10">
         <v>210.43439669875249</v>
       </c>
-      <c r="P33" s="11">
+      <c r="Q33" s="11">
         <v>2.60703922607658</v>
       </c>
-      <c r="Q33" s="7">
-        <f>P33/O33</f>
+      <c r="R33" s="7">
+        <f>Q33/P33</f>
         <v>1.2388845488072413E-2</v>
       </c>
-      <c r="R33" s="10">
+      <c r="S33" s="10">
         <v>294.60367481420053</v>
       </c>
-      <c r="S33" s="10">
+      <c r="T33" s="10">
         <v>798.47919893728385</v>
       </c>
-      <c r="T33" s="6">
-        <f>SUM(O33:S33)</f>
+      <c r="U33" s="6">
+        <f>SUM(P33:T33)</f>
         <v>1306.1366985218015</v>
       </c>
-      <c r="U33" s="5">
-        <f>R33/T33</f>
+      <c r="V33" s="5">
+        <f>S33/U33</f>
         <v>0.22555347778499246</v>
       </c>
-      <c r="V33" s="5">
-        <f>O33/T33</f>
+      <c r="W33" s="5">
+        <f>P33/U33</f>
         <v>0.16111207727101468</v>
       </c>
-      <c r="W33" s="5">
-        <f>S33/T33</f>
+      <c r="X33" s="5">
+        <f>T33/U33</f>
         <v>0.61132896720607377</v>
       </c>
-      <c r="X33" s="5">
-        <f>S33/T33</f>
+      <c r="Y33" s="5">
+        <f>T33/U33</f>
         <v>0.61132896720607377</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>18</v>
       </c>
@@ -2044,23 +2061,28 @@
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="4">
+      <c r="K34" s="5">
+        <v>729.33658076210634</v>
+      </c>
+      <c r="L34" s="5">
         <v>45.080000000000005</v>
       </c>
-      <c r="L34" s="5">
+      <c r="M34" s="5">
         <v>328.78493060755761</v>
       </c>
-      <c r="M34" s="4"/>
-      <c r="N34" s="8">
+      <c r="N34" s="5">
+        <v>400.55165015454872</v>
+      </c>
+      <c r="O34" s="5">
         <v>14.483917647910022</v>
       </c>
-      <c r="P34" s="8"/>
       <c r="Q34" s="8"/>
-      <c r="Y34" s="8">
+      <c r="R34" s="8"/>
+      <c r="Z34" s="8">
         <v>136.9</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
@@ -2087,10 +2109,10 @@
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-      <c r="M35" s="4"/>
-      <c r="Y35" s="8"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K35" s="5"/>
+      <c r="Z35" s="8"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>19</v>
       </c>
@@ -2114,45 +2136,36 @@
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="M36" s="9"/>
-      <c r="O36" s="10">
+      <c r="K36" s="5"/>
+      <c r="N36" s="11"/>
+      <c r="P36" s="10">
         <v>5.8937500000000007</v>
       </c>
-      <c r="P36" s="11">
+      <c r="Q36" s="11">
         <v>5.9718750000000001E-2</v>
       </c>
-      <c r="Q36" s="7">
-        <f>P36/O36</f>
+      <c r="R36" s="7">
+        <f>Q36/P36</f>
         <v>1.013255567338282E-2</v>
       </c>
-      <c r="R36" s="10">
+      <c r="S36" s="10">
         <v>2.3125</v>
       </c>
-      <c r="S36" s="10">
-        <v>0</v>
-      </c>
-      <c r="T36" s="6">
-        <f>SUM(O36:S36)</f>
+      <c r="T36" s="10"/>
+      <c r="U36" s="6">
+        <f>SUM(P36:T36)</f>
         <v>8.2761013056733823</v>
       </c>
-      <c r="U36" s="5">
-        <f>R36/T36</f>
+      <c r="V36" s="5">
+        <f>S36/U36</f>
         <v>0.27941900595329217</v>
       </c>
-      <c r="V36" s="5">
-        <f>O36/T36</f>
+      <c r="W36" s="5">
+        <f>P36/U36</f>
         <v>0.71214087192960696</v>
       </c>
-      <c r="W36" s="5">
-        <f>S36/T36</f>
-        <v>0</v>
-      </c>
-      <c r="X36" s="5">
-        <f>S36/T36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>19</v>
       </c>
@@ -2174,8 +2187,9 @@
       <c r="J37" s="2">
         <v>5.875</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>19</v>
       </c>
@@ -2197,8 +2211,9 @@
       <c r="J38" s="2">
         <v>9.25</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>19</v>
       </c>
@@ -2225,45 +2240,46 @@
       </c>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
-      <c r="M39" s="9"/>
-      <c r="O39" s="10">
+      <c r="K39" s="5"/>
+      <c r="N39" s="11"/>
+      <c r="P39" s="10">
         <v>31.950000000000003</v>
       </c>
-      <c r="P39" s="11">
+      <c r="Q39" s="11">
         <v>0.47235625000000003</v>
       </c>
-      <c r="Q39" s="7">
-        <f>P39/O39</f>
+      <c r="R39" s="7">
+        <f>Q39/P39</f>
         <v>1.478423317683881E-2</v>
       </c>
-      <c r="R39" s="10">
+      <c r="S39" s="10">
         <v>22.337499999999999</v>
       </c>
-      <c r="S39" s="10">
+      <c r="T39" s="10">
         <v>1.8435726463606257</v>
       </c>
-      <c r="T39" s="6">
-        <f>SUM(O39:S39)</f>
+      <c r="U39" s="6">
+        <f>SUM(P39:T39)</f>
         <v>56.618213129537466</v>
       </c>
-      <c r="U39" s="5">
-        <f>R39/T39</f>
+      <c r="V39" s="5">
+        <f>S39/U39</f>
         <v>0.39452852298418134</v>
       </c>
-      <c r="V39" s="5">
-        <f>O39/T39</f>
+      <c r="W39" s="5">
+        <f>P39/U39</f>
         <v>0.56430604630529801</v>
       </c>
-      <c r="W39" s="5">
-        <f>S39/T39</f>
+      <c r="X39" s="5">
+        <f>T39/U39</f>
         <v>3.2561477031122381E-2</v>
       </c>
-      <c r="X39" s="5">
-        <f>S39/T39</f>
+      <c r="Y39" s="5">
+        <f>T39/U39</f>
         <v>3.2561477031122381E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>19</v>
       </c>
@@ -2285,8 +2301,9 @@
       <c r="J40" s="2">
         <v>14.125</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>19</v>
       </c>
@@ -2317,45 +2334,46 @@
       <c r="J41" s="2">
         <v>15.574999999999999</v>
       </c>
-      <c r="M41" s="9"/>
-      <c r="O41" s="10">
+      <c r="K41" s="1"/>
+      <c r="N41" s="11"/>
+      <c r="P41" s="10">
         <v>97.636296673003514</v>
       </c>
-      <c r="P41" s="11">
+      <c r="Q41" s="11">
         <v>1.576929912123707</v>
       </c>
-      <c r="Q41" s="7">
-        <f>P41/O41</f>
+      <c r="R41" s="7">
+        <f>Q41/P41</f>
         <v>1.6151062318607266E-2</v>
       </c>
-      <c r="R41" s="10">
+      <c r="S41" s="10">
         <v>119.34398983755042</v>
       </c>
-      <c r="S41" s="10">
+      <c r="T41" s="10">
         <v>11.061435878163755</v>
       </c>
-      <c r="T41" s="6">
-        <f>SUM(O41:S41)</f>
+      <c r="U41" s="6">
+        <f>SUM(P41:T41)</f>
         <v>229.63480336316002</v>
       </c>
-      <c r="U41" s="5">
-        <f>R41/T41</f>
+      <c r="V41" s="5">
+        <f>S41/U41</f>
         <v>0.51971211719510901</v>
       </c>
-      <c r="V41" s="5">
-        <f>O41/T41</f>
+      <c r="W41" s="5">
+        <f>P41/U41</f>
         <v>0.42518074456943211</v>
       </c>
-      <c r="W41" s="5">
-        <f>S41/T41</f>
+      <c r="X41" s="5">
+        <f>T41/U41</f>
         <v>4.81696838465311E-2</v>
       </c>
-      <c r="X41" s="5">
-        <f>S41/T41</f>
+      <c r="Y41" s="5">
+        <f>T41/U41</f>
         <v>4.81696838465311E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>19</v>
       </c>
@@ -2377,8 +2395,9 @@
       <c r="J42" s="2">
         <v>16.625</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>19</v>
       </c>
@@ -2400,8 +2419,9 @@
       <c r="J43" s="2">
         <v>19.25</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>19</v>
       </c>
@@ -2425,45 +2445,46 @@
       </c>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
-      <c r="M44" s="9"/>
-      <c r="O44" s="10">
+      <c r="K44" s="5"/>
+      <c r="N44" s="11"/>
+      <c r="P44" s="10">
         <v>178.43939986556762</v>
       </c>
-      <c r="P44" s="11">
+      <c r="Q44" s="11">
         <v>3.0477266722548508</v>
       </c>
-      <c r="Q44" s="7">
-        <f>P44/O44</f>
+      <c r="R44" s="7">
+        <f>Q44/P44</f>
         <v>1.7079897570553039E-2</v>
       </c>
-      <c r="R44" s="10">
+      <c r="S44" s="10">
         <v>226.94069596341399</v>
       </c>
-      <c r="S44" s="10">
+      <c r="T44" s="10">
         <v>91.519673052504658</v>
       </c>
-      <c r="T44" s="6">
-        <f>SUM(O44:S44)</f>
+      <c r="U44" s="6">
+        <f>SUM(P44:T44)</f>
         <v>499.9645754513117</v>
       </c>
-      <c r="U44" s="5">
-        <f>R44/T44</f>
+      <c r="V44" s="5">
+        <f>S44/U44</f>
         <v>0.45391355129222405</v>
       </c>
-      <c r="V44" s="5">
-        <f>O44/T44</f>
+      <c r="W44" s="5">
+        <f>P44/U44</f>
         <v>0.35690408606348284</v>
       </c>
-      <c r="W44" s="5">
-        <f>S44/T44</f>
+      <c r="X44" s="5">
+        <f>T44/U44</f>
         <v>0.18305231519631368</v>
       </c>
-      <c r="X44" s="5">
-        <f>S44/T44</f>
+      <c r="Y44" s="5">
+        <f>T44/U44</f>
         <v>0.18305231519631368</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>19</v>
       </c>
@@ -2485,8 +2506,9 @@
       <c r="J45" s="2">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>19</v>
       </c>
@@ -2508,8 +2530,9 @@
       <c r="J46" s="2">
         <v>23.475000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>19</v>
       </c>
@@ -2536,45 +2559,46 @@
       </c>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
-      <c r="M47" s="9"/>
-      <c r="O47" s="10">
+      <c r="K47" s="5"/>
+      <c r="N47" s="11"/>
+      <c r="P47" s="10">
         <v>214.45780535823133</v>
       </c>
-      <c r="P47" s="11">
+      <c r="Q47" s="11">
         <v>3.5873690971259045</v>
       </c>
-      <c r="Q47" s="7">
-        <f>P47/O47</f>
+      <c r="R47" s="7">
+        <f>Q47/P47</f>
         <v>1.6727621972693167E-2</v>
       </c>
-      <c r="R47" s="10">
+      <c r="S47" s="10">
         <v>282.47894443387111</v>
       </c>
-      <c r="S47" s="10">
+      <c r="T47" s="10">
         <v>303.64106075122243</v>
       </c>
-      <c r="T47" s="6">
-        <f>SUM(O47:S47)</f>
+      <c r="U47" s="6">
+        <f>SUM(P47:T47)</f>
         <v>804.18190726242346</v>
       </c>
-      <c r="U47" s="5">
-        <f>R47/T47</f>
+      <c r="V47" s="5">
+        <f>S47/U47</f>
         <v>0.35126249656060915</v>
       </c>
-      <c r="V47" s="5">
-        <f>O47/T47</f>
+      <c r="W47" s="5">
+        <f>P47/U47</f>
         <v>0.26667822717907619</v>
       </c>
-      <c r="W47" s="5">
-        <f>S47/T47</f>
+      <c r="X47" s="5">
+        <f>T47/U47</f>
         <v>0.37757758289398718</v>
       </c>
-      <c r="X47" s="5">
-        <f>S47/T47</f>
+      <c r="Y47" s="5">
+        <f>T47/U47</f>
         <v>0.37757758289398718</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>19</v>
       </c>
@@ -2596,8 +2620,9 @@
       <c r="J48" s="2">
         <v>24.774999999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>19</v>
       </c>
@@ -2624,45 +2649,46 @@
       </c>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
-      <c r="M49" s="9"/>
-      <c r="O49" s="10">
+      <c r="K49" s="5"/>
+      <c r="N49" s="11"/>
+      <c r="P49" s="10">
         <v>216.82420168274621</v>
       </c>
-      <c r="P49" s="11">
+      <c r="Q49" s="11">
         <v>3.8612415248064167</v>
       </c>
-      <c r="Q49" s="7">
-        <f>P49/O49</f>
+      <c r="R49" s="7">
+        <f>Q49/P49</f>
         <v>1.7808166684529642E-2</v>
       </c>
-      <c r="R49" s="10">
+      <c r="S49" s="10">
         <v>325.46560562045931</v>
       </c>
-      <c r="S49" s="10">
+      <c r="T49" s="10">
         <v>589.92479634008544</v>
       </c>
-      <c r="T49" s="6">
-        <f>SUM(O49:S49)</f>
+      <c r="U49" s="6">
+        <f>SUM(P49:T49)</f>
         <v>1136.0936533347817</v>
       </c>
-      <c r="U49" s="5">
-        <f>R49/T49</f>
+      <c r="V49" s="5">
+        <f>S49/U49</f>
         <v>0.28647779579185079</v>
       </c>
-      <c r="V49" s="5">
-        <f>O49/T49</f>
+      <c r="W49" s="5">
+        <f>P49/U49</f>
         <v>0.19085064074277766</v>
       </c>
-      <c r="W49" s="5">
-        <f>S49/T49</f>
+      <c r="X49" s="5">
+        <f>T49/U49</f>
         <v>0.51925718853236791</v>
       </c>
-      <c r="X49" s="5">
-        <f>S49/T49</f>
+      <c r="Y49" s="5">
+        <f>T49/U49</f>
         <v>0.51925718853236791</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>19</v>
       </c>
@@ -2689,45 +2715,46 @@
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
-      <c r="M50" s="9"/>
-      <c r="O50" s="10">
+      <c r="K50" s="5"/>
+      <c r="N50" s="11"/>
+      <c r="P50" s="10">
         <v>167.79349020251826</v>
       </c>
-      <c r="P50" s="11">
+      <c r="Q50" s="11">
         <v>2.419173051724484</v>
       </c>
-      <c r="Q50" s="7">
-        <f>P50/O50</f>
+      <c r="R50" s="7">
+        <f>Q50/P50</f>
         <v>1.441756202105734E-2</v>
       </c>
-      <c r="R50" s="10">
+      <c r="S50" s="10">
         <v>353.23362452520678</v>
       </c>
-      <c r="S50" s="10">
+      <c r="T50" s="10">
         <v>753.59700414609051</v>
       </c>
-      <c r="T50" s="6">
-        <f>SUM(O50:S50)</f>
+      <c r="U50" s="6">
+        <f>SUM(P50:T50)</f>
         <v>1277.0577094875612</v>
       </c>
-      <c r="U50" s="5">
-        <f>R50/T50</f>
+      <c r="V50" s="5">
+        <f>S50/U50</f>
         <v>0.27659957878250241</v>
       </c>
-      <c r="V50" s="5">
-        <f>O50/T50</f>
+      <c r="W50" s="5">
+        <f>P50/U50</f>
         <v>0.13139068732441853</v>
       </c>
-      <c r="W50" s="5">
-        <f>S50/T50</f>
+      <c r="X50" s="5">
+        <f>T50/U50</f>
         <v>0.59010411083809422</v>
       </c>
-      <c r="X50" s="5">
-        <f>S50/T50</f>
+      <c r="Y50" s="5">
+        <f>T50/U50</f>
         <v>0.59010411083809422</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>19</v>
       </c>
@@ -2754,19 +2781,24 @@
       </c>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
-      <c r="K51" s="4">
+      <c r="K51" s="5">
+        <v>485.63373045382281</v>
+      </c>
+      <c r="L51" s="5">
         <v>44.080000000000005</v>
       </c>
-      <c r="L51" s="5">
+      <c r="M51" s="5">
         <v>214.06734838404515</v>
       </c>
-      <c r="M51" s="4"/>
-      <c r="N51" s="8">
+      <c r="N51" s="5">
+        <v>271.56638206977766</v>
+      </c>
+      <c r="O51" s="5">
         <v>9.4302796644953784</v>
       </c>
-      <c r="P51" s="8"/>
       <c r="Q51" s="8"/>
-      <c r="Y51" s="8">
+      <c r="R51" s="8"/>
+      <c r="Z51" s="8">
         <v>126.3</v>
       </c>
     </row>
@@ -2779,7 +2811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D514C363-0C51-48C9-B03D-3EAE5BBC25DE}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>